<commit_message>
Bug fixes for exception handling and validaiton of Excel report
</commit_message>
<xml_diff>
--- a/Config/App-Repo-Mapping.xlsx
+++ b/Config/App-Repo-Mapping.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CAST\Development\VSCode\GitRepo\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CAST\Development\VSCode\CASTHLAutomation\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FA56D0-8BB3-48E2-ACDB-7099873FA750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD976356-95F8-4C78-8038-6ECECB348474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35865" yWindow="3645" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="App-Repo-Mapping" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>Application</t>
   </si>
@@ -40,9 +40,6 @@
     <t>com.castsoftware.labs.jee.missingtable</t>
   </si>
   <si>
-    <t>App1</t>
-  </si>
-  <si>
     <t>com.castsoftware.uc.imsdc</t>
   </si>
   <si>
@@ -73,13 +70,13 @@
     <t>Template</t>
   </si>
   <si>
-    <t>App2</t>
-  </si>
-  <si>
-    <t>App3</t>
-  </si>
-  <si>
-    <t>App4</t>
+    <t>Demo</t>
+  </si>
+  <si>
+    <t>BeverageStarterFlow</t>
+  </si>
+  <si>
+    <t>Demo-Brio</t>
   </si>
 </sst>
 </file>
@@ -948,7 +945,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -965,7 +964,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -973,7 +972,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -981,7 +980,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -989,7 +988,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -1000,7 +999,7 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -1008,7 +1007,7 @@
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -1016,7 +1015,7 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -1024,7 +1023,7 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -1032,7 +1031,7 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -1040,7 +1039,7 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -1048,31 +1047,31 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>